<commit_message>
feat: se añaden objetivos, indicadores y límites
</commit_message>
<xml_diff>
--- a/cmi.xlsx
+++ b/cmi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maksi\Documentos\cmi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maksi\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,236 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+  <si>
+    <t>Cantidad de presupuestos</t>
+  </si>
+  <si>
+    <t>Ingresos de limpiezas de PC</t>
+  </si>
+  <si>
+    <t>Costos de componentes</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Financiera</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Crecimiento y Aprendizaje</t>
+  </si>
+  <si>
+    <t>Procesos internos</t>
+  </si>
+  <si>
+    <t>Área de incidencia</t>
+  </si>
+  <si>
+    <t>Nombre del indicador</t>
+  </si>
+  <si>
+    <t>Aumentar cantidad de presupuestos</t>
+  </si>
+  <si>
+    <t>Aumentar ingresos de limpiezas de PC</t>
+  </si>
+  <si>
+    <t>Reducir costos de componentes para repuesto</t>
+  </si>
+  <si>
+    <t>Aumentar ingresos de clientes</t>
+  </si>
+  <si>
+    <t>Ingresos de clientes</t>
+  </si>
+  <si>
+    <t>Reducir cantidad de quejas</t>
+  </si>
+  <si>
+    <t>Cantidad de quejas </t>
+  </si>
+  <si>
+    <t>Aumentar frecuencia de clientes</t>
+  </si>
+  <si>
+    <t>Frecuencia de clientes</t>
+  </si>
+  <si>
+    <t>Aumentar cantidad de clientes por servicios</t>
+  </si>
+  <si>
+    <t>Cantidad de clientes por servicio</t>
+  </si>
+  <si>
+    <t>Reducir de tiempo de entrega de PC</t>
+  </si>
+  <si>
+    <t>Tiempo de entrega</t>
+  </si>
+  <si>
+    <t>Aumentar presupuesto anual del local para componentes</t>
+  </si>
+  <si>
+    <t>Presupuesto del local para componenetes</t>
+  </si>
+  <si>
+    <t>Aumentar presupuesto anual de herramientas</t>
+  </si>
+  <si>
+    <t>Presupuesto del local para herramientas</t>
+  </si>
+  <si>
+    <t>Aumentar capacitación de empleados</t>
+  </si>
+  <si>
+    <t>Cantidad de capacitaciones</t>
+  </si>
+  <si>
+    <t>Aumentar horas de capacitación</t>
+  </si>
+  <si>
+    <t>Horas de capacitación</t>
+  </si>
+  <si>
+    <t>Aumentar cantidad de empleados</t>
+  </si>
+  <si>
+    <t>Cantidad de empleados</t>
+  </si>
+  <si>
+    <t>&gt; 50 presupuestos</t>
+  </si>
+  <si>
+    <t>&lt; 10%</t>
+  </si>
+  <si>
+    <t>&lt; 5 quejas</t>
+  </si>
+  <si>
+    <t>&gt; 20 clientes</t>
+  </si>
+  <si>
+    <t>&gt; 15 clientes</t>
+  </si>
+  <si>
+    <t>&lt; 2 días</t>
+  </si>
+  <si>
+    <t>&gt; 12 capacitaciones</t>
+  </si>
+  <si>
+    <t>&gt; 100 horas</t>
+  </si>
+  <si>
+    <t>&gt; 30 empleados</t>
+  </si>
+  <si>
+    <t>30 - 50 presupuestos</t>
+  </si>
+  <si>
+    <t>&lt; 30 presupuestos</t>
+  </si>
+  <si>
+    <t>10% - 20%</t>
+  </si>
+  <si>
+    <t>&gt; 20%</t>
+  </si>
+  <si>
+    <t>5 - 10 quejas</t>
+  </si>
+  <si>
+    <t>&gt; 10 quejas</t>
+  </si>
+  <si>
+    <t>10 - 20 clientes</t>
+  </si>
+  <si>
+    <t>&lt; 10 clientes</t>
+  </si>
+  <si>
+    <t>10 - 15 clientes</t>
+  </si>
+  <si>
+    <t>2 - 4 días</t>
+  </si>
+  <si>
+    <t>&gt; 4 días</t>
+  </si>
+  <si>
+    <t>6 - 12 capacitaciones</t>
+  </si>
+  <si>
+    <t>&lt; 6 capacitaciones</t>
+  </si>
+  <si>
+    <t>50 - 100 horas</t>
+  </si>
+  <si>
+    <t>&lt; 50 horas</t>
+  </si>
+  <si>
+    <t>15 - 30 empleados</t>
+  </si>
+  <si>
+    <t>&lt; 15 empleados</t>
+  </si>
+  <si>
+    <t>Límite verde</t>
+  </si>
+  <si>
+    <t>Límite amarillo</t>
+  </si>
+  <si>
+    <t>Límite rojo</t>
+  </si>
+  <si>
+    <t>&lt; $400.000</t>
+  </si>
+  <si>
+    <t>&gt; $600.000</t>
+  </si>
+  <si>
+    <t>$600.000 - $400.000</t>
+  </si>
+  <si>
+    <t>&gt; $1.500.000</t>
+  </si>
+  <si>
+    <t>$1.500.000 - $1.000.000</t>
+  </si>
+  <si>
+    <t>&lt; $100.000.000</t>
+  </si>
+  <si>
+    <t>&gt; $20.000.000</t>
+  </si>
+  <si>
+    <t>$20.000.000 - $15.000.000</t>
+  </si>
+  <si>
+    <t>&lt; $15.000.000</t>
+  </si>
+  <si>
+    <t>&gt; $5.000.000</t>
+  </si>
+  <si>
+    <t>$5.000.000 - $3.000.0000</t>
+  </si>
+  <si>
+    <t>&lt; $3.000.000</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +260,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -50,18 +335,402 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FF99FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -336,12 +1005,434 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11">
+      <c r="C3" s="53"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" ht="25.5">
+      <c r="B6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" ht="45.75" thickBot="1">
+      <c r="B7" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" ht="27" thickTop="1" thickBot="1">
+      <c r="B8" s="46"/>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" ht="27" thickTop="1" thickBot="1">
+      <c r="B9" s="46"/>
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" ht="26.25" thickTop="1">
+      <c r="B10" s="47"/>
+      <c r="C10" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" ht="31.5" thickTop="1" thickBot="1">
+      <c r="B12" s="34"/>
+      <c r="C12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" ht="30.75" thickTop="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" ht="26.25" thickBot="1">
+      <c r="B14" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" ht="31.5" thickTop="1" thickBot="1">
+      <c r="B15" s="31"/>
+      <c r="C15" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" ht="26.25" thickTop="1">
+      <c r="B16" s="32"/>
+      <c r="C16" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" ht="30.75" thickBot="1">
+      <c r="B17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" ht="27" thickTop="1" thickBot="1">
+      <c r="B18" s="7"/>
+      <c r="C18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" ht="30.75" thickTop="1">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="4"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="4"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="4"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="4"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: se añade pestaña con gráfico para un indicador
Junto con fórmulas desordenadas.
</commit_message>
<xml_diff>
--- a/cmi.xlsx
+++ b/cmi.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maksi\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maksi\Documentos\cmi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Componentes" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
   <si>
     <t>Cantidad de presupuestos</t>
   </si>
@@ -246,13 +247,73 @@
   </si>
   <si>
     <t>&lt; $3.000.000</t>
+  </si>
+  <si>
+    <t>Doughnut Chart</t>
+  </si>
+  <si>
+    <t>Pie Chart</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Pointer Settings</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Pointer</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>&gt; $40.000.000</t>
+  </si>
+  <si>
+    <t>$40.000.000 - $15.000.000</t>
+  </si>
+  <si>
+    <t>Rojo</t>
+  </si>
+  <si>
+    <t>Amarillo</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Valor actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +355,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,8 +405,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -557,11 +648,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -577,145 +716,180 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,6 +914,1327 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Componentes!$G$3</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4451010853373058"/>
+          <c:y val="2.5089605734767026E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21551343910958495"/>
+          <c:y val="0.15437262096164681"/>
+          <c:w val="0.60874849525388275"/>
+          <c:h val="0.84562737903835317"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13213213213213215"/>
+                  <c:y val="-4.6594982078853112E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Componentes!$A$3</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Poor</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{FC5DAFC3-2B2F-4299-B52A-1260CD7875CF}</c15:txfldGUID>
+                      <c15:f>Componentes!$A$3</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>Poor</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11111111111111113"/>
+                  <c:y val="-8.9605734767025089E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Componentes!$A$4</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{B3DAD581-EC06-4692-944F-FAA2958CE993}</c15:txfldGUID>
+                      <c15:f>Componentes!$A$4</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5054419061708078E-17"/>
+                  <c:y val="-0.13620071684587814"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Componentes!$A$5</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Good</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{10F991EB-5E19-4FB0-A1E2-A60D69DD7029}</c15:txfldGUID>
+                      <c15:f>Componentes!$A$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>Good</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13213213213213212"/>
+                  <c:y val="-8.6021505376344093E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Componentes!$A$6</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{1D4297AE-918F-4783-B1AC-6FE42292F753}</c15:txfldGUID>
+                      <c15:f>Componentes!$A$6</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15015015015015015"/>
+                  <c:y val="-5.0179211469534114E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Componentes!$A$7</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Excellent</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{5086D37D-D490-4601-B581-B0D94D1DDEEF}</c15:txfldGUID>
+                      <c15:f>Componentes!$A$7</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>Excellent</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-2E3D-4321-A6B7-9B176E4D4E03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Componentes!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-2E3D-4321-A6B7-9B176E4D4E03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="270"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-2E3D-4321-A6B7-9B176E4D4E03}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Componentes!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>189</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>Pointer</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-2E3D-4321-A6B7-9B176E4D4E03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="270"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>36195</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{084E1343-8A84-446C-98D3-63ECA07C20C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.47387</cdr:x>
+      <cdr:y>0.62981</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.69355</cdr:x>
+      <cdr:y>0.73088</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="Componentes!$B$28">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62782D53-83C6-4A78-A85B-4649035A644A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1958907" y="2562736"/>
+          <a:ext cx="908118" cy="411262"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fld id="{30CBA863-4B3A-4A51-9E5A-72739FB4BBC0}" type="TxLink">
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>8.000.000</a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="1800" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1005,10 +2500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K36"/>
+  <dimension ref="B3:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1021,7 +2516,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
-      <c r="C3" s="53"/>
+      <c r="C3" s="41"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
@@ -1037,219 +2532,219 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:11" ht="25.5">
-      <c r="B6" s="48" t="s">
+    <row r="6" spans="2:11">
+      <c r="B6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="40" t="s">
         <v>61</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="2:11" ht="45.75" thickBot="1">
-      <c r="B7" s="45" t="s">
+    <row r="7" spans="2:11" ht="26.25" thickBot="1">
+      <c r="B7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="29" t="s">
         <v>43</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B8" s="46"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="17" t="s">
         <v>62</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B9" s="46"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B10" s="47"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="31" t="s">
         <v>67</v>
       </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="34" t="s">
         <v>47</v>
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="2:11" ht="31.5" thickTop="1" thickBot="1">
-      <c r="B12" s="34"/>
-      <c r="C12" s="23" t="s">
+    <row r="12" spans="2:11" ht="27" thickTop="1" thickBot="1">
+      <c r="B12" s="46"/>
+      <c r="C12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="39" t="s">
         <v>49</v>
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:11" ht="30.75" thickTop="1">
-      <c r="B13" s="35"/>
-      <c r="C13" s="23" t="s">
+    <row r="13" spans="2:11" ht="26.25" thickTop="1">
+      <c r="B13" s="47"/>
+      <c r="C13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="34" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="2:11" ht="26.25" thickBot="1">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="24" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="2:11" ht="31.5" thickTop="1" thickBot="1">
-      <c r="B15" s="31"/>
-      <c r="C15" s="25" t="s">
+    <row r="15" spans="2:11" ht="27" thickTop="1" thickBot="1">
+      <c r="B15" s="49"/>
+      <c r="C15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="24" t="s">
         <v>70</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B16" s="32"/>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="24" t="s">
         <v>73</v>
       </c>
       <c r="H16" s="2"/>
@@ -1257,23 +2752,23 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="2:11" ht="30.75" thickBot="1">
-      <c r="B17" s="29" t="s">
+    <row r="17" spans="2:11" ht="26.25" thickBot="1">
+      <c r="B17" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="14" t="s">
         <v>54</v>
       </c>
       <c r="H17" s="2"/>
@@ -1282,20 +2777,20 @@
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B18" s="7"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="10" t="s">
         <v>56</v>
       </c>
       <c r="H18" s="2"/>
@@ -1303,21 +2798,21 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="2:11" ht="30.75" thickTop="1">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
+    <row r="19" spans="2:11" ht="26.25" thickTop="1">
+      <c r="B19" s="53"/>
+      <c r="C19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="2"/>
@@ -1354,76 +2849,80 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="5"/>
+      <c r="B25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="5"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="4"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="5"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="61"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="5"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="61"/>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="4"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="63"/>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="4"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="5"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1435,4 +2934,240 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="17" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="57"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="59">
+        <v>18.75</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="59">
+        <f>B28/E25*100</f>
+        <v>10</v>
+      </c>
+      <c r="F3" s="57"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="60"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="61">
+        <v>1</v>
+      </c>
+      <c r="F4" s="57"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="59">
+        <v>31.25</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="63">
+        <f>200-(E3+E4)</f>
+        <v>189</v>
+      </c>
+      <c r="F5" s="57"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="60"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="59">
+        <v>50</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="65">
+        <v>100</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+    </row>
+    <row r="15" spans="1:17" ht="30">
+      <c r="M15" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="P15" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q15" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="30">
+      <c r="M16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q16" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="66">
+        <v>15000000</v>
+      </c>
+      <c r="C25" s="66">
+        <v>25000000</v>
+      </c>
+      <c r="D25" s="66">
+        <v>40000000</v>
+      </c>
+      <c r="E25" s="66">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26">
+        <f>B25/E25*100</f>
+        <v>18.75</v>
+      </c>
+      <c r="C26">
+        <f>C25/E25*100</f>
+        <v>31.25</v>
+      </c>
+      <c r="D26">
+        <f>D25/E25*100</f>
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <f>SUM(B26:D26)</f>
+        <v>100</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="66">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: boceto de indicador de presupuesto
</commit_message>
<xml_diff>
--- a/cmi.xlsx
+++ b/cmi.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maksi\Documentos\cmi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos de programa\xampp\htdocs\cmi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C137700-B124-41A2-BF0C-13A2DC42FA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Componentes" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Componentes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
   <si>
     <t>Cantidad de presupuestos</t>
   </si>
@@ -307,12 +309,51 @@
   </si>
   <si>
     <t>Valor actual</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Presupuestos (2024)</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Presupuesto (2023)</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -700,12 +741,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -715,7 +755,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -819,42 +858,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,31 +868,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,7 +959,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -972,7 +1012,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1142,10 +1182,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FC5DAFC3-2B2F-4299-B52A-1260CD7875CF}</c15:txfldGUID>
+                      <c15:txfldGUID>{485D2AA6-EB19-49F8-9B64-F52B87D92528}</c15:txfldGUID>
                       <c15:f>Componentes!$A$3</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1186,10 +1225,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B3DAD581-EC06-4692-944F-FAA2958CE993}</c15:txfldGUID>
+                      <c15:txfldGUID>{5E11529F-9864-4501-B143-EC48977D5AFD}</c15:txfldGUID>
                       <c15:f>Componentes!$A$4</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1230,10 +1268,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{10F991EB-5E19-4FB0-A1E2-A60D69DD7029}</c15:txfldGUID>
+                      <c15:txfldGUID>{062B917A-3915-4022-8F87-4180B72F8F78}</c15:txfldGUID>
                       <c15:f>Componentes!$A$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1274,10 +1311,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{1D4297AE-918F-4783-B1AC-6FE42292F753}</c15:txfldGUID>
+                      <c15:txfldGUID>{A7B5FA54-F06D-46A9-AA53-BD14D033A617}</c15:txfldGUID>
                       <c15:f>Componentes!$A$6</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1318,10 +1354,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5086D37D-D490-4601-B581-B0D94D1DDEEF}</c15:txfldGUID>
+                      <c15:txfldGUID>{081E4F78-ADF0-4D51-80D4-6973B3CC6BE3}</c15:txfldGUID>
                       <c15:f>Componentes!$A$7</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1374,7 +1409,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1494,13 +1529,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>43.958333333333336</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>189</c:v>
+                  <c:v>155.04166666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1539,7 +1574,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1547,6 +1581,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1570,7 +1605,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2188,12 +2223,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.47387</cdr:x>
-      <cdr:y>0.62981</cdr:y>
+      <cdr:x>0.36664</cdr:x>
+      <cdr:y>0.60777</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.69355</cdr:x>
-      <cdr:y>0.73088</cdr:y>
+      <cdr:x>0.66752</cdr:x>
+      <cdr:y>0.70884</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="Componentes!$B$28">
       <cdr:nvSpPr>
@@ -2208,8 +2243,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1958907" y="2562736"/>
-          <a:ext cx="908118" cy="411262"/>
+          <a:off x="1514729" y="2443451"/>
+          <a:ext cx="1243090" cy="406336"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2220,16 +2255,167 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fld id="{30CBA863-4B3A-4A51-9E5A-72739FB4BBC0}" type="TxLink">
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>8.000.000</a:t>
+            <a:pPr/>
+            <a:t>35.166.667</a:t>
           </a:fld>
-          <a:endParaRPr lang="en-US" sz="1800" b="1"/>
+          <a:endParaRPr lang="en-US" sz="3200" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.27612</cdr:x>
+      <cdr:y>0.82295</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84446</cdr:x>
+      <cdr:y>0.92212</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89BD4D51-BB63-8CC3-2F61-0AE8BA192E5B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1140785" y="3308541"/>
+          <a:ext cx="2348023" cy="398721"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="es-AR" sz="1800"/>
+            <a:t>Objetivo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1800" baseline="0"/>
+            <a:t>: 50.000.000</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.07664</cdr:x>
+      <cdr:y>0.05396</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.97855</cdr:x>
+      <cdr:y>0.15313</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDB69BB-E353-F586-14B6-7D658EADB6DA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="316613" y="216934"/>
+          <a:ext cx="3726195" cy="398721"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="es-AR" sz="1600" baseline="0"/>
+            <a:t>Aumentar presupuestos de componentes</a:t>
+          </a:r>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2499,14 +2685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -2515,414 +2701,361 @@
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
-      <c r="C3" s="41"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="36" t="s">
+    <row r="3" spans="2:7">
+      <c r="C3" s="39"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" ht="26.25" thickBot="1">
-      <c r="B7" s="42" t="s">
+    </row>
+    <row r="7" spans="2:7" ht="26.25" thickBot="1">
+      <c r="B7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B8" s="43"/>
-      <c r="C8" s="19" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="27" thickTop="1" thickBot="1">
+      <c r="B8" s="54"/>
+      <c r="C8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B9" s="43"/>
-      <c r="C9" s="19" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="27" thickTop="1" thickBot="1">
+      <c r="B9" s="54"/>
+      <c r="C9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B10" s="44"/>
-      <c r="C10" s="28" t="s">
+    </row>
+    <row r="10" spans="2:7" ht="26.25" thickTop="1">
+      <c r="B10" s="55"/>
+      <c r="C10" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B11" s="45" t="s">
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B11" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B12" s="46"/>
-      <c r="C12" s="21" t="s">
+    </row>
+    <row r="12" spans="2:7" ht="27" thickTop="1" thickBot="1">
+      <c r="B12" s="57"/>
+      <c r="C12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B13" s="47"/>
-      <c r="C13" s="21" t="s">
+    </row>
+    <row r="13" spans="2:7" ht="26.25" thickTop="1">
+      <c r="B13" s="58"/>
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" ht="26.25" thickBot="1">
-      <c r="B14" s="48" t="s">
+    </row>
+    <row r="14" spans="2:7" ht="26.25" thickBot="1">
+      <c r="B14" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B15" s="49"/>
-      <c r="C15" s="23" t="s">
+    </row>
+    <row r="15" spans="2:7" ht="31.5" thickTop="1" thickBot="1">
+      <c r="B15" s="60"/>
+      <c r="C15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B16" s="50"/>
-      <c r="C16" s="22" t="s">
+    </row>
+    <row r="16" spans="2:7" ht="26.25" thickTop="1">
+      <c r="B16" s="61"/>
+      <c r="C16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" ht="26.25" thickBot="1">
-      <c r="B17" s="51" t="s">
+    </row>
+    <row r="17" spans="2:9" ht="30.75" thickBot="1">
+      <c r="B17" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" ht="27" thickTop="1" thickBot="1">
-      <c r="B18" s="52"/>
-      <c r="C18" s="9" t="s">
+    </row>
+    <row r="18" spans="2:9" ht="27" thickTop="1" thickBot="1">
+      <c r="B18" s="63"/>
+      <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" ht="26.25" thickTop="1">
-      <c r="B19" s="53"/>
-      <c r="C19" s="7" t="s">
+    </row>
+    <row r="19" spans="2:9" ht="26.25" thickTop="1">
+      <c r="B19" s="64"/>
+      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="4"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="2:11">
-      <c r="B25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
-    </row>
-    <row r="27" spans="2:11">
-      <c r="B27" s="58"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="59"/>
-    </row>
-    <row r="28" spans="2:11">
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
-    </row>
-    <row r="29" spans="2:11">
-      <c r="B29" s="58"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="59"/>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="61"/>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="B31" s="58"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="63"/>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="64"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="46"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="47"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="47"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="49"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2937,17 +3070,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27449F7F-F70B-49D7-A6E9-3B1CEA4FBCAA}">
+  <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" ht="25.5">
+      <c r="B3" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="E13" sqref="B13:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
@@ -2961,146 +3170,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="57"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="45">
         <v>18.75</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="45">
         <f>B28/E25*100</f>
-        <v>10</v>
-      </c>
-      <c r="F3" s="57"/>
+        <v>43.958333333333336</v>
+      </c>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="60" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="61">
+      <c r="E4" s="47">
         <v>1</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="45">
         <v>31.25</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="62" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="49">
         <f>200-(E3+E4)</f>
-        <v>189</v>
-      </c>
-      <c r="F5" s="57"/>
+        <v>155.04166666666666</v>
+      </c>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="60"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="45">
         <v>50</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="51">
         <v>100</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="15" spans="1:17" ht="30">
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="N15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="P15" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="Q15" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30">
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="24" t="s">
+      <c r="O16" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="P16" s="24" t="s">
+      <c r="P16" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Q16" s="24" t="s">
+      <c r="Q16" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:5">
       <c r="B24" t="s">
         <v>88</v>
       </c>
@@ -3114,24 +3323,24 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="66">
+      <c r="B25" s="52">
         <v>15000000</v>
       </c>
-      <c r="C25" s="66">
+      <c r="C25" s="52">
         <v>25000000</v>
       </c>
-      <c r="D25" s="66">
+      <c r="D25" s="52">
         <v>40000000</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="52">
         <v>80000000</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -3151,19 +3360,75 @@
         <f>SUM(B26:D26)</f>
         <v>100</v>
       </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="28" spans="1:8">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="66">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="B28" s="52">
+        <f>SUM(B33:B38)/COUNT(B33:B38)</f>
+        <v>35166666.666666664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="65">
+        <v>30000000</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="65">
+        <v>1000000</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="65">
+        <v>10000000</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="65">
+        <v>90000000</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="65">
+        <v>50000000</v>
+      </c>
+      <c r="C37" s="65" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="65">
+        <v>30000000</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>